<commit_message>
Fix twoColumn form to use the correct form_id
</commit_message>
<xml_diff>
--- a/app/tables/twoColumn/forms/twoColumn/twoColumn.xlsx
+++ b/app/tables/twoColumn/forms/twoColumn/twoColumn.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="6360" windowWidth="25820" windowHeight="16220"/>
+    <workbookView xWindow="1920" yWindow="6360" windowWidth="25820" windowHeight="16220" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -294,9 +294,6 @@
     <t>display.image</t>
   </si>
   <si>
-    <t>twoColulmn</t>
-  </si>
-  <si>
     <t>Two Column Form</t>
   </si>
   <si>
@@ -313,6 +310,9 @@
   </si>
   <si>
     <t>assign</t>
+  </si>
+  <si>
+    <t>twoColumn</t>
   </si>
 </sst>
 </file>
@@ -674,32 +674,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="24.453125" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="40.81640625" customWidth="1"/>
-    <col min="5" max="6" width="17.36328125" customWidth="1"/>
-    <col min="7" max="8" width="27.1796875" customWidth="1"/>
-    <col min="9" max="9" width="24.81640625" customWidth="1"/>
-    <col min="10" max="10" width="41.81640625" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" customWidth="1"/>
+    <col min="5" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="8" width="27.1640625" customWidth="1"/>
+    <col min="9" max="9" width="24.83203125" customWidth="1"/>
+    <col min="10" max="10" width="41.83203125" customWidth="1"/>
     <col min="11" max="11" width="40" customWidth="1"/>
-    <col min="12" max="12" width="14.36328125" customWidth="1"/>
-    <col min="13" max="13" width="20.453125" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="13" max="13" width="20.5" customWidth="1"/>
     <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="15.81640625" customWidth="1"/>
-    <col min="16" max="16" width="18.36328125" customWidth="1"/>
-    <col min="17" max="17" width="18.453125" customWidth="1"/>
+    <col min="15" max="15" width="15.83203125" customWidth="1"/>
+    <col min="16" max="16" width="18.33203125" customWidth="1"/>
+    <col min="17" max="17" width="18.5" customWidth="1"/>
     <col min="18" max="18" width="19" customWidth="1"/>
     <col min="21" max="21" width="27" customWidth="1"/>
-    <col min="22" max="22" width="15.1796875" customWidth="1"/>
+    <col min="22" max="22" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:22" ht="17.5" customHeight="1">
       <c r="B1" t="s">
         <v>82</v>
       </c>
@@ -710,10 +710,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
@@ -761,16 +761,16 @@
         <v>9</v>
       </c>
       <c r="V1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="2:22" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="2:22" ht="17.5" customHeight="1">
       <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="2:22" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:22" ht="17.5" customHeight="1">
       <c r="F3">
         <v>1</v>
       </c>
@@ -787,7 +787,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:22" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22" ht="17.5" customHeight="1">
       <c r="C4" t="s">
         <v>83</v>
       </c>
@@ -801,7 +801,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="2:22" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22" ht="17.5" customHeight="1">
       <c r="F5">
         <v>2</v>
       </c>
@@ -818,7 +818,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:22" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22" ht="17.5" customHeight="1">
       <c r="C6" t="s">
         <v>84</v>
       </c>
@@ -830,23 +830,23 @@
       <c r="I6" s="1"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="2:22" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22" ht="17.5" customHeight="1">
       <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="2:22" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:22" ht="17.5" customHeight="1">
       <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H8" s="1"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="2:22" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22" ht="17.5" customHeight="1">
       <c r="F9">
         <v>1</v>
       </c>
@@ -861,7 +861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:22" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:22" ht="17.5" customHeight="1">
       <c r="F10">
         <v>2</v>
       </c>
@@ -885,7 +885,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:22" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:22" ht="17.5" customHeight="1">
       <c r="F11">
         <v>1</v>
       </c>
@@ -902,7 +902,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:22" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" ht="17.5" customHeight="1">
       <c r="F12">
         <v>2</v>
       </c>
@@ -917,17 +917,17 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="2:22" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22" ht="17.5" customHeight="1">
       <c r="C13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H13" s="1"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="2:22" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22" ht="17.5" customHeight="1">
       <c r="C14" s="1"/>
       <c r="G14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
@@ -938,7 +938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:22" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:22" ht="17.5" customHeight="1">
       <c r="G15" s="1" t="s">
         <v>14</v>
       </c>
@@ -962,98 +962,98 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:22" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:22" ht="17.5" customHeight="1"/>
+    <row r="17" ht="17.5" customHeight="1"/>
+    <row r="18" ht="17.5" customHeight="1"/>
+    <row r="19" ht="17.5" customHeight="1"/>
+    <row r="20" ht="17.5" customHeight="1"/>
+    <row r="21" ht="17.5" customHeight="1"/>
+    <row r="22" ht="17.5" customHeight="1"/>
+    <row r="23" ht="17.5" customHeight="1"/>
+    <row r="24" ht="17.5" customHeight="1"/>
+    <row r="25" ht="17.5" customHeight="1"/>
+    <row r="26" ht="17.5" customHeight="1"/>
+    <row r="27" ht="17.5" customHeight="1"/>
+    <row r="28" ht="17.5" customHeight="1"/>
+    <row r="29" ht="17.5" customHeight="1"/>
+    <row r="30" ht="17.5" customHeight="1"/>
+    <row r="31" ht="17.5" customHeight="1"/>
+    <row r="32" ht="17.5" customHeight="1"/>
+    <row r="33" ht="17.5" customHeight="1"/>
+    <row r="34" ht="17.5" customHeight="1"/>
+    <row r="35" ht="17.5" customHeight="1"/>
+    <row r="36" ht="17.5" customHeight="1"/>
+    <row r="37" ht="17.5" customHeight="1"/>
+    <row r="38" ht="17.5" customHeight="1"/>
+    <row r="39" ht="17.5" customHeight="1"/>
+    <row r="40" ht="17.5" customHeight="1"/>
+    <row r="41" ht="17.5" customHeight="1"/>
+    <row r="42" ht="17.5" customHeight="1"/>
+    <row r="43" ht="17.5" customHeight="1"/>
+    <row r="44" ht="17.5" customHeight="1"/>
+    <row r="45" ht="17.5" customHeight="1"/>
+    <row r="46" ht="17.5" customHeight="1"/>
+    <row r="47" ht="17.5" customHeight="1"/>
+    <row r="48" ht="17.5" customHeight="1"/>
+    <row r="49" ht="17.5" customHeight="1"/>
+    <row r="50" ht="17.5" customHeight="1"/>
+    <row r="51" ht="17.5" customHeight="1"/>
+    <row r="52" ht="17.5" customHeight="1"/>
+    <row r="53" ht="17.5" customHeight="1"/>
+    <row r="54" ht="17.5" customHeight="1"/>
+    <row r="55" ht="17.5" customHeight="1"/>
+    <row r="56" ht="17.5" customHeight="1"/>
+    <row r="57" ht="17.5" customHeight="1"/>
+    <row r="58" ht="17.5" customHeight="1"/>
+    <row r="59" ht="17.5" customHeight="1"/>
+    <row r="60" ht="17.5" customHeight="1"/>
+    <row r="61" ht="17.5" customHeight="1"/>
+    <row r="62" ht="17.5" customHeight="1"/>
+    <row r="63" ht="17.5" customHeight="1"/>
+    <row r="64" ht="17.5" customHeight="1"/>
+    <row r="65" ht="17.5" customHeight="1"/>
+    <row r="66" ht="17.5" customHeight="1"/>
+    <row r="67" ht="17.5" customHeight="1"/>
+    <row r="68" ht="17.5" customHeight="1"/>
+    <row r="69" ht="17.5" customHeight="1"/>
+    <row r="70" ht="17.5" customHeight="1"/>
+    <row r="71" ht="17.5" customHeight="1"/>
+    <row r="72" ht="17.5" customHeight="1"/>
+    <row r="73" ht="17.5" customHeight="1"/>
+    <row r="74" ht="17.5" customHeight="1"/>
+    <row r="75" ht="17.5" customHeight="1"/>
+    <row r="76" ht="17.5" customHeight="1"/>
+    <row r="77" ht="17.5" customHeight="1"/>
+    <row r="78" ht="17.5" customHeight="1"/>
+    <row r="79" ht="17.5" customHeight="1"/>
+    <row r="80" ht="17.5" customHeight="1"/>
+    <row r="81" ht="17.5" customHeight="1"/>
+    <row r="82" ht="17.5" customHeight="1"/>
+    <row r="83" ht="17.5" customHeight="1"/>
+    <row r="84" ht="17.5" customHeight="1"/>
+    <row r="85" ht="17.5" customHeight="1"/>
+    <row r="86" ht="17.5" customHeight="1"/>
+    <row r="87" ht="17.5" customHeight="1"/>
+    <row r="88" ht="17.5" customHeight="1"/>
+    <row r="89" ht="17.5" customHeight="1"/>
+    <row r="90" ht="17.5" customHeight="1"/>
+    <row r="91" ht="17.5" customHeight="1"/>
+    <row r="92" ht="17.5" customHeight="1"/>
+    <row r="93" ht="17.5" customHeight="1"/>
+    <row r="94" ht="17.5" customHeight="1"/>
+    <row r="95" ht="17.5" customHeight="1"/>
+    <row r="96" ht="17.5" customHeight="1"/>
+    <row r="97" ht="17.5" customHeight="1"/>
+    <row r="98" ht="17.5" customHeight="1"/>
+    <row r="99" ht="17.5" customHeight="1"/>
+    <row r="100" ht="17.5" customHeight="1"/>
+    <row r="101" ht="17.5" customHeight="1"/>
+    <row r="102" ht="17.5" customHeight="1"/>
+    <row r="103" ht="17.5" customHeight="1"/>
+    <row r="104" ht="17.5" customHeight="1"/>
+    <row r="105" ht="17.5" customHeight="1"/>
+    <row r="106" ht="17.5" customHeight="1"/>
+    <row r="107" ht="17.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1072,13 +1072,13 @@
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.453125" customWidth="1"/>
-    <col min="2" max="2" width="49.453125" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="49.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="17.5" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>77</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="17.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
@@ -1112,14 +1112,14 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.81640625" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" customWidth="1"/>
-    <col min="3" max="3" width="23.453125" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="17.5" customHeight="1">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="17.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="17.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="17.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="17.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="17.5" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="17.5" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="17.5" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="17.5" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="17.5" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
@@ -1229,8 +1229,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="17.5" customHeight="1"/>
+    <row r="12" spans="1:3" ht="17.5" customHeight="1">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="17.5" customHeight="1">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="17.5" customHeight="1">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="17.5" customHeight="1">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="17.5" customHeight="1">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="17.5" customHeight="1">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="17.5" customHeight="1">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="17.5" customHeight="1">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="17.5" customHeight="1">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="17.5" customHeight="1">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1340,8 +1340,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="17.5" customHeight="1"/>
+    <row r="23" spans="1:3" ht="17.5" customHeight="1">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="17.5" customHeight="1">
       <c r="A24" t="s">
         <v>67</v>
       </c>
@@ -1363,8 +1363,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:3" ht="17.5" customHeight="1"/>
+    <row r="26" spans="1:3" ht="17.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1379,18 +1379,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.453125" customWidth="1"/>
-    <col min="2" max="2" width="24.1796875" customWidth="1"/>
-    <col min="3" max="3" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="14.5" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>74</v>
       </c>
@@ -1401,15 +1401,15 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="14.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
@@ -1417,17 +1417,17 @@
         <v>20130408</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="14.5" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>86</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14.5" customHeight="1"/>
+    <row r="6" spans="1:3" ht="14.5" customHeight="1"/>
+    <row r="7" spans="1:3" ht="14.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>